<commit_message>
Updated Excel file TestDataNew and created a data Provider for login functionality
</commit_message>
<xml_diff>
--- a/meritnations/src/test/resources/TestDataNew.xlsx
+++ b/meritnations/src/test/resources/TestDataNew.xlsx
@@ -27,10 +27,10 @@
     <t>sunaina@test.com</t>
   </si>
   <si>
-    <t>Reproduce Steps</t>
+    <t>Display Name</t>
   </si>
   <si>
-    <t xml:space="preserve">1.)Enter valid Username and valid password                 2.) Click Login Button     </t>
+    <t>Sunaina</t>
   </si>
 </sst>
 </file>
@@ -379,11 +379,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>

</xml_diff>